<commit_message>
Added a a step to calculate protein meal and re-ran the pipeline. lsmeans seem to have been calculated without issue.
Also added protein meal to the phenotype name conversion utility tables.
</commit_message>
<xml_diff>
--- a/data/utils/trait_name_lookup.xlsx
+++ b/data/utils/trait_name_lookup.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jay\Documents\R\Projects\Jay_yield\data\utils\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jhgille2\Documents\R\projects\Jay_yield\data\utils\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{73A57361-5696-4304-9514-FD9980D71CF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF800DF8-4AC3-4666-A6F2-D59E0D159870}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1610" yWindow="8820" windowWidth="14620" windowHeight="9450" xr2:uid="{F874549B-2F4E-41DC-AF60-06FD0551DD83}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F874549B-2F4E-41DC-AF60-06FD0551DD83}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>md</t>
   </si>
@@ -95,6 +95,12 @@
   </si>
   <si>
     <t>trait_name</t>
+  </si>
+  <si>
+    <t>protein_meal</t>
+  </si>
+  <si>
+    <t>Protein Meal</t>
   </si>
 </sst>
 </file>
@@ -446,15 +452,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14DF6AF7-5DAD-49B4-BDF1-B70E11EDF326}">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>19</v>
       </c>
@@ -462,7 +468,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -470,7 +476,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -478,7 +484,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -486,7 +492,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -494,7 +500,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -502,7 +508,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -510,7 +516,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -518,7 +524,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -526,12 +532,20 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
       <c r="B10" t="s">
         <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added functions to make and export summplmental data tables. Replaced the function that exported the contrast supplemental table with this new one that exports all the supplemental tables and moved the code to make the contrast supplemental table to the new function that makes the other tables.
Also changed the plot export function a bit to explicitly export the correlation plots as supplemental figure and added protein meal to the correlation figures.

SOme other small changes to the manuscript document to add a formula for protein meal and fix some references that weren't properly rendering.
</commit_message>
<xml_diff>
--- a/data/utils/trait_name_lookup.xlsx
+++ b/data/utils/trait_name_lookup.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jhgille2\Documents\R\projects\Jay_yield\data\utils\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF800DF8-4AC3-4666-A6F2-D59E0D159870}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF83CBC1-D1A9-4941-82EB-74AD1BD591E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F874549B-2F4E-41DC-AF60-06FD0551DD83}"/>
+    <workbookView xWindow="-25290" yWindow="600" windowWidth="14310" windowHeight="15600" xr2:uid="{F874549B-2F4E-41DC-AF60-06FD0551DD83}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -85,9 +85,6 @@
     <t>Yield (bu/ac)</t>
   </si>
   <si>
-    <t>Seeed Weight (grams)</t>
-  </si>
-  <si>
     <t>Seed Quality</t>
   </si>
   <si>
@@ -101,6 +98,9 @@
   </si>
   <si>
     <t>Protein Meal</t>
+  </si>
+  <si>
+    <t>Seed Weight (grams)</t>
   </si>
 </sst>
 </file>
@@ -455,14 +455,14 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B1" t="s">
         <v>9</v>
@@ -521,7 +521,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -529,7 +529,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -537,15 +537,15 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" t="s">
         <v>20</v>
-      </c>
-      <c r="B11" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>